<commit_message>
update TAN in ENA plant sample extension template
</commit_message>
<xml_diff>
--- a/templates/dataplant/ENA/ENA_-_Plant_sample_-_extension.xlsx
+++ b/templates/dataplant/ENA/ENA_-_Plant_sample_-_extension.xlsx
@@ -32,7 +32,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.0.1</t>
   </si>
   <si>
     <t>Description</t>
@@ -275,10 +275,10 @@
     <t>Characteristic [organism common name]</t>
   </si>
   <si>
-    <t>Term Source REF (OBI:0100026)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (OBI:0100026)</t>
+    <t>Term Source REF (OBI:0003074)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (OBI:0003074)</t>
   </si>
   <si>
     <t>Characteristic [subspecific genetic lineage rank]</t>
@@ -603,8 +603,8 @@
     <tableColumn id="27" name="Term Source REF (DPBO:0000032)" totalsRowFunction="none"/>
     <tableColumn id="28" name="Term Accession Number (DPBO:0000032)" totalsRowFunction="none"/>
     <tableColumn id="29" name="Characteristic [organism common name]" totalsRowFunction="none"/>
-    <tableColumn id="30" name="Term Source REF (OBI:0100026)" totalsRowFunction="none"/>
-    <tableColumn id="31" name="Term Accession Number (OBI:0100026)" totalsRowFunction="none"/>
+    <tableColumn id="30" name="Term Source REF (OBI:0003074)" totalsRowFunction="none"/>
+    <tableColumn id="31" name="Term Accession Number (OBI:0003074)" totalsRowFunction="none"/>
     <tableColumn id="32" name="Characteristic [subspecific genetic lineage rank]" totalsRowFunction="none"/>
     <tableColumn id="33" name="Term Source REF (DPBO:0000037)" totalsRowFunction="none"/>
     <tableColumn id="34" name="Term Accession Number (DPBO:0000037)" totalsRowFunction="none"/>

</xml_diff>